<commit_message>
Update on 20200731 part 4
</commit_message>
<xml_diff>
--- a/文档/其他文档/Others/PC/20200803开始的新工作作息.xlsx
+++ b/文档/其他文档/Others/PC/20200803开始的新工作作息.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="48">
   <si>
     <t>Monday</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -88,10 +88,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>面试时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>上下午都可</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -166,11 +162,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>整理需求测试的需求
-并发送测试计划邮件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>下午若遇面试：
 可晚上到家后发送测试计划邮件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -193,6 +184,35 @@
   </si>
   <si>
     <t>如若邮件在周五之前未反馈，需要去催促确认</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当日工作侧重于</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求（下午）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可安排面试时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>等待需求反馈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>整理要测试的需求
+并发送测试计划邮件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -223,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,12 +265,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,8 +292,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -302,19 +328,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -329,11 +378,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,17 +699,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -669,7 +732,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -679,46 +742,46 @@
       <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="5" t="s">
-        <v>13</v>
+      <c r="F3" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -729,17 +792,17 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -748,45 +811,67 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="12" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="10" t="s">
-        <v>38</v>
+      <c r="D9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B4:F4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -796,17 +881,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -832,15 +917,15 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="7"/>
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -848,38 +933,40 @@
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="9"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -888,38 +975,54 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="12" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="10" t="s">
-        <v>38</v>
+      <c r="D8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -948,89 +1051,89 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>34</v>
+      <c r="C2" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>34</v>
+        <v>22</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>31</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="13" t="s">
         <v>32</v>
       </c>
+      <c r="C6" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="D7" s="2"/>
     </row>

</xml_diff>

<commit_message>
Update on 20200731 part 5
</commit_message>
<xml_diff>
--- a/文档/其他文档/Others/PC/20200803开始的新工作作息.xlsx
+++ b/文档/其他文档/Others/PC/20200803开始的新工作作息.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="49">
   <si>
     <t>Monday</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,11 +75,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>提交需求
-反馈文档</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Noon</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -213,6 +208,16 @@
   <si>
     <t>整理要测试的需求
 并发送测试计划邮件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如若邮件在周五之前未反馈，需要去催促确认
+如若甘路、赵哲豪在周五下午2点半-3点仍未反馈，则默认按照"按计划实施"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提交需求反馈文档
+并发送上线计划邮件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -381,21 +386,21 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -732,7 +737,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -750,29 +755,29 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -792,7 +797,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -800,71 +805,71 @@
         <v>11</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="D8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>44</v>
+      <c r="F8" s="14" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="D9" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -931,15 +936,15 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -964,65 +969,65 @@
         <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>44</v>
+      <c r="D7" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="15" t="s">
-        <v>44</v>
+      <c r="F7" s="14" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1051,44 +1056,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>24</v>
-      </c>
       <c r="C2" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1097,43 +1102,43 @@
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>40</v>
+      <c r="D5" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="D7" s="2"/>
     </row>

</xml_diff>